<commit_message>
feat: 2d vs 3d
</commit_message>
<xml_diff>
--- a/data/arange/00_olds/01_all_params/220208 IDs.xlsx
+++ b/data/arange/00_olds/01_all_params/220208 IDs.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yosuke_shibata/04_laboratory/04_part_time/01_code/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yosuke_shibata/Documents/03_labo/03_part_time/01_irides_kyoto/data/arange/00_olds/01_all_params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB01C1D1-7AE8-5441-A47F-C6BD1D248919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE88F9E-1D45-184D-BBBC-6FAD664CA88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="result" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -813,7 +814,7 @@
   <dimension ref="A1:EH31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B39" sqref="B35:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>